<commit_message>
Website Automation for sprint 4 CRMF-165
</commit_message>
<xml_diff>
--- a/Data Files/API/CRM/API_Ninja_Van.xlsx
+++ b/Data Files/API/CRM/API_Ninja_Van.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
+    <workbookView windowWidth="18650" windowHeight="7110" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="API_Ninja_Van_Dev" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="36">
   <si>
     <t>shipper_id</t>
   </si>
@@ -95,7 +95,7 @@
     <t>Van en-route to pickup</t>
   </si>
   <si>
-    <t>10466</t>
+    <t>10001545</t>
   </si>
   <si>
     <t>SG-Singapore-Ninja Van Sorting Facility</t>
@@ -119,7 +119,10 @@
     <t>https://link.to/pod.jpeg</t>
   </si>
   <si>
-    <t>10001270</t>
+    <t>10001547</t>
+  </si>
+  <si>
+    <t>10001558</t>
   </si>
 </sst>
 </file>
@@ -128,9 +131,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -165,7 +168,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,7 +197,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -187,83 +220,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,11 +244,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -294,187 +297,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,13 +491,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -539,30 +546,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -580,6 +563,26 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -590,157 +593,154 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
@@ -1070,55 +1070,55 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="22.1111111111111" customWidth="1"/>
-    <col min="3" max="3" width="18.5555555555556" customWidth="1"/>
-    <col min="4" max="4" width="19.1111111111111" customWidth="1"/>
-    <col min="5" max="5" width="24.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="25.8888888888889" customWidth="1"/>
-    <col min="7" max="7" width="38.5555555555556" customWidth="1"/>
-    <col min="8" max="8" width="21.5555555555556" customWidth="1"/>
-    <col min="9" max="9" width="14.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="22.1090909090909" customWidth="1"/>
+    <col min="3" max="3" width="18.5545454545455" customWidth="1"/>
+    <col min="4" max="4" width="19.1090909090909" customWidth="1"/>
+    <col min="5" max="5" width="24.6636363636364" customWidth="1"/>
+    <col min="6" max="6" width="25.8909090909091" customWidth="1"/>
+    <col min="7" max="7" width="38.5545454545455" customWidth="1"/>
+    <col min="8" max="8" width="21.5545454545455" customWidth="1"/>
+    <col min="9" max="9" width="14.6636363636364" customWidth="1"/>
     <col min="10" max="10" width="36" customWidth="1"/>
-    <col min="11" max="11" width="18.1111111111111" customWidth="1"/>
+    <col min="11" max="11" width="18.1090909090909" customWidth="1"/>
     <col min="12" max="12" width="27" customWidth="1"/>
-    <col min="13" max="13" width="25.8888888888889" customWidth="1"/>
+    <col min="13" max="13" width="25.8909090909091" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="9.77777777777778" customWidth="1"/>
-    <col min="16" max="16" width="19.6666666666667" customWidth="1"/>
-    <col min="17" max="17" width="11.6666666666667" customWidth="1"/>
-    <col min="18" max="18" width="22.1111111111111" customWidth="1"/>
-    <col min="19" max="19" width="21.5555555555556" customWidth="1"/>
+    <col min="15" max="15" width="9.78181818181818" customWidth="1"/>
+    <col min="16" max="16" width="19.6636363636364" customWidth="1"/>
+    <col min="17" max="17" width="11.6636363636364" customWidth="1"/>
+    <col min="18" max="18" width="22.1090909090909" customWidth="1"/>
+    <col min="19" max="19" width="21.5545454545455" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -1158,68 +1158,128 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:19">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:19">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="2">
         <v>9987976</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="3" t="b">
+      <c r="S2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>9987976</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="2" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" display="https://link.to/pod.jpeg"/>
+    <hyperlink ref="R3" r:id="rId1" display="https://link.to/pod.jpeg"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1229,156 +1289,276 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="22.1111111111111" customWidth="1"/>
-    <col min="3" max="3" width="18.5555555555556" customWidth="1"/>
-    <col min="4" max="4" width="19.1111111111111" customWidth="1"/>
-    <col min="5" max="5" width="24.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="25.8888888888889" customWidth="1"/>
-    <col min="7" max="7" width="38.5555555555556" customWidth="1"/>
-    <col min="8" max="8" width="21.5555555555556" customWidth="1"/>
-    <col min="9" max="9" width="14.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="22.1090909090909" customWidth="1"/>
+    <col min="3" max="3" width="18.5545454545455" customWidth="1"/>
+    <col min="4" max="4" width="19.1090909090909" customWidth="1"/>
+    <col min="5" max="5" width="24.6636363636364" customWidth="1"/>
+    <col min="6" max="6" width="25.8909090909091" customWidth="1"/>
+    <col min="7" max="7" width="38.5545454545455" customWidth="1"/>
+    <col min="8" max="8" width="21.5545454545455" customWidth="1"/>
+    <col min="9" max="9" width="14.6636363636364" customWidth="1"/>
     <col min="10" max="10" width="36" customWidth="1"/>
-    <col min="11" max="11" width="18.1111111111111" customWidth="1"/>
+    <col min="11" max="11" width="18.1090909090909" customWidth="1"/>
     <col min="12" max="12" width="27" customWidth="1"/>
-    <col min="13" max="13" width="25.8888888888889" customWidth="1"/>
+    <col min="13" max="13" width="25.8909090909091" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="9.77777777777778" customWidth="1"/>
-    <col min="16" max="16" width="19.6666666666667" customWidth="1"/>
-    <col min="17" max="17" width="11.6666666666667" customWidth="1"/>
-    <col min="18" max="18" width="22.1111111111111" customWidth="1"/>
-    <col min="19" max="19" width="21.5555555555556" customWidth="1"/>
+    <col min="15" max="15" width="9.78181818181818" customWidth="1"/>
+    <col min="16" max="16" width="19.6636363636364" customWidth="1"/>
+    <col min="17" max="17" width="11.6636363636364" customWidth="1"/>
+    <col min="18" max="18" width="22.1090909090909" customWidth="1"/>
+    <col min="19" max="19" width="21.5545454545455" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:19">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:19">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>9987976</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q3" s="2">
         <v>9987976</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="3" t="b">
+      <c r="S3" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>9987976</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="2" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" display="https://link.to/pod.jpeg"/>
+    <hyperlink ref="R3" r:id="rId1" display="https://link.to/pod.jpeg"/>
+    <hyperlink ref="R4" r:id="rId1" display="https://link.to/pod.jpeg"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Website Update Automation Leads
</commit_message>
<xml_diff>
--- a/Data Files/API/CRM/API_Ninja_Van.xlsx
+++ b/Data Files/API/CRM/API_Ninja_Van.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
   <si>
     <t>shipper_id</t>
   </si>
@@ -95,7 +95,7 @@
     <t>Van en-route to pickup</t>
   </si>
   <si>
-    <t>10001545</t>
+    <t xml:space="preserve"> 10994</t>
   </si>
   <si>
     <t>SG-Singapore-Ninja Van Sorting Facility</t>
@@ -117,12 +117,6 @@
   </si>
   <si>
     <t>https://link.to/pod.jpeg</t>
-  </si>
-  <si>
-    <t>10001547</t>
-  </si>
-  <si>
-    <t>10001558</t>
   </si>
 </sst>
 </file>
@@ -130,12 +124,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +138,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10.5"/>
+      <color rgb="FF5F6368"/>
+      <name val="Roboto"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -152,38 +152,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color rgb="FF4D4D4D"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,8 +174,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,25 +221,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,45 +280,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,187 +303,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,21 +494,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -516,16 +507,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -546,16 +537,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -588,20 +579,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -611,134 +617,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -748,8 +754,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1070,13 +1080,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="22.1090909090909" customWidth="1"/>
@@ -1088,7 +1098,7 @@
     <col min="8" max="8" width="21.5545454545455" customWidth="1"/>
     <col min="9" max="9" width="14.6636363636364" customWidth="1"/>
     <col min="10" max="10" width="36" customWidth="1"/>
-    <col min="11" max="11" width="18.1090909090909" customWidth="1"/>
+    <col min="11" max="11" width="25.3636363636364" customWidth="1"/>
     <col min="12" max="12" width="27" customWidth="1"/>
     <col min="13" max="13" width="25.8909090909091" customWidth="1"/>
     <col min="14" max="14" width="12" customWidth="1"/>
@@ -1192,7 +1202,7 @@
       <c r="K2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="5" t="s">
         <v>29</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -1210,7 +1220,7 @@
       <c r="Q2" s="2">
         <v>9987976</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="4" t="s">
         <v>33</v>
       </c>
       <c r="S2" s="2" t="b">
@@ -1218,68 +1228,35 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>9987976</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="11:11">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="7" spans="11:11">
+      <c r="K7" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" display="https://link.to/pod.jpeg"/>
-    <hyperlink ref="R3" r:id="rId1" display="https://link.to/pod.jpeg"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
@@ -1291,8 +1268,8 @@
   <sheetPr/>
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89090909090909" defaultRowHeight="14.5" outlineLevelRow="3"/>
@@ -1402,8 +1379,8 @@
       <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>26</v>
+      <c r="I2" s="3">
+        <v>10001862</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>27</v>
@@ -1429,7 +1406,7 @@
       <c r="Q2" s="2">
         <v>9987976</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="4" t="s">
         <v>33</v>
       </c>
       <c r="S2" s="2" t="b">
@@ -1461,8 +1438,8 @@
       <c r="H3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>34</v>
+      <c r="I3" s="3">
+        <v>10001863</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>27</v>
@@ -1488,7 +1465,7 @@
       <c r="Q3" s="2">
         <v>9987976</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="S3" s="2" t="b">
@@ -1496,69 +1473,30 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>9987976</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S4" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="R2" r:id="rId1" display="https://link.to/pod.jpeg"/>
     <hyperlink ref="R3" r:id="rId1" display="https://link.to/pod.jpeg"/>
-    <hyperlink ref="R4" r:id="rId1" display="https://link.to/pod.jpeg"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>